<commit_message>
implemented type split by cohort, made total cal vs val graphs
</commit_message>
<xml_diff>
--- a/Data/cleaned_and_combined_data/Type_Split/Type_Split_ratios.xlsx
+++ b/Data/cleaned_and_combined_data/Type_Split/Type_Split_ratios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,34 +434,137 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Age classes</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>SFH_ratio</t>
+          <t>% SFH</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>TH_ratio</t>
+          <t>% TH</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>AB_ratio</t>
+          <t>% AB</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1955 and before</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5222</v>
+        <v>0.5542353624916999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2062</v>
+        <v>0.1977404405643929</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2716</v>
+        <v>0.2480241969439072</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>1956 - 1970</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5290045118645327</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1893335251958855</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2816619629395818</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>1971 - 1980</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.5726899924657374</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1890630662102659</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2382469413239968</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>1981 - 1990</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6122221616745076</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2137909529604805</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1739868853650119</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>1991 - 2000</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.476144176678936</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2414751024376693</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2823807208833947</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2001 - 2010</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.336760881642224</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.2304784821084705</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4327606362493056</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2011 and after</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.340234951214744</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2475518509961434</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4122131977891126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>